<commit_message>
Finished the order statistics
</commit_message>
<xml_diff>
--- a/xlsx/pdf.xlsx
+++ b/xlsx/pdf.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A78"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,391 +433,627 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>bins</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>-0.147</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>-0.147</v>
+        <v>-0.1445</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>-0.1445</v>
+        <v>-0.142</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>-0.142</v>
+        <v>-0.1395</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>-0.1395</v>
+        <v>-0.137</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>-0.137</v>
+        <v>-0.1345</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>-0.1345</v>
+        <v>-0.132</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>-0.132</v>
+        <v>-0.1295</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>-0.1295</v>
+        <v>-0.127</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>-0.127</v>
+        <v>-0.1245</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>-0.1245</v>
+        <v>-0.122</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>-0.122</v>
+        <v>-0.1195</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>-0.1195</v>
+        <v>-0.117</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>-0.117</v>
+        <v>-0.1145</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>-0.1145</v>
+        <v>-0.112</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>-0.112</v>
+        <v>-0.1095</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>-0.1095</v>
+        <v>-0.107</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>-0.107</v>
+        <v>-0.1045</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>-0.1045</v>
+        <v>-0.102</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>-0.102</v>
+        <v>-0.09950000000000001</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>-0.09949999999999995</v>
+        <v>-0.097</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>-0.09699999999999995</v>
+        <v>-0.0945</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>-0.09449999999999995</v>
+        <v>-0.092</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>-0.09199999999999994</v>
+        <v>-0.0895</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>-0.08949999999999994</v>
+        <v>-0.08699999999999999</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>-0.08699999999999994</v>
+        <v>-0.08450000000000001</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>-0.08449999999999994</v>
+        <v>-0.082</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>-0.08199999999999993</v>
+        <v>-0.0795</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>-0.07949999999999993</v>
+        <v>-0.077</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>-0.07699999999999993</v>
+        <v>-0.0745</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>-0.07449999999999993</v>
+        <v>-0.07199999999999999</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>-0.07199999999999993</v>
+        <v>-0.06950000000000001</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>-0.06949999999999992</v>
+        <v>-0.067</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>-0.06699999999999992</v>
+        <v>-0.0645</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>-0.06449999999999992</v>
+        <v>-0.062</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>-0.06199999999999992</v>
+        <v>-0.0595</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>-0.05949999999999991</v>
+        <v>-0.057</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>-0.05699999999999991</v>
+        <v>-0.0545</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>-0.05449999999999991</v>
+        <v>-0.052</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>-0.05199999999999991</v>
+        <v>-0.0495</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>-0.04949999999999991</v>
+        <v>-0.047</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>-0.0469999999999999</v>
+        <v>-0.0445</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>-0.0444999999999999</v>
+        <v>-0.042</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>-0.0419999999999999</v>
+        <v>-0.0395</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>-0.0394999999999999</v>
+        <v>-0.037</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>-0.03699999999999989</v>
+        <v>-0.0345</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>-0.03449999999999989</v>
+        <v>-0.032</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>-0.03199999999999989</v>
+        <v>-0.0295</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>-0.02949999999999989</v>
+        <v>-0.027</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>-0.02699999999999989</v>
+        <v>-0.0245</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>-0.02449999999999988</v>
+        <v>-0.022</v>
+      </c>
+      <c r="B52" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>-0.02199999999999988</v>
+        <v>-0.0195</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>-0.01949999999999988</v>
+        <v>-0.017</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>-0.01699999999999988</v>
+        <v>-0.0145</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>-0.01449999999999987</v>
+        <v>-0.012</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>-0.01199999999999987</v>
+        <v>-0.0095</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>-0.00949999999999987</v>
+        <v>-0.007</v>
+      </c>
+      <c r="B58" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>-0.006999999999999867</v>
+        <v>-0.0045</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>-0.004499999999999865</v>
+        <v>-0.002</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>-0.001999999999999863</v>
+        <v>0.0005</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>0.0005000000000001392</v>
+        <v>0.003</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>0.003000000000000141</v>
+        <v>0.0055</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>0.005500000000000144</v>
+        <v>0.008</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>0.008000000000000146</v>
+        <v>0.0105</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>0.01050000000000015</v>
+        <v>0.013</v>
+      </c>
+      <c r="B66" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>0.01300000000000015</v>
+        <v>0.0155</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>0.01550000000000015</v>
+        <v>0.018</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>0.01800000000000015</v>
+        <v>0.0205</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>0.02050000000000016</v>
+        <v>0.023</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>0.02300000000000016</v>
+        <v>0.0255</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>0.02550000000000016</v>
+        <v>0.028</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>0.02800000000000016</v>
+        <v>0.0305</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>0.03050000000000017</v>
+        <v>0.033</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>0.03300000000000017</v>
+        <v>0.0355</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>0.03550000000000017</v>
+        <v>0.038</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>0.03800000000000017</v>
+        <v>0.0405</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>0.04050000000000017</v>
+        <v>0.043</v>
+      </c>
+      <c r="B78" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Looped the download. Needs fixing
</commit_message>
<xml_diff>
--- a/xlsx/pdf.xlsx
+++ b/xlsx/pdf.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,7 +442,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>-0.147</v>
+        <v>-0.36</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -450,7 +450,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>-0.1445</v>
+        <v>-0.3575</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -458,7 +458,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>-0.142</v>
+        <v>-0.355</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>-0.1395</v>
+        <v>-0.3525</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>-0.137</v>
+        <v>-0.35</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>-0.1345</v>
+        <v>-0.3475</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -490,7 +490,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>-0.132</v>
+        <v>-0.345</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>-0.1295</v>
+        <v>-0.3425</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>-0.127</v>
+        <v>-0.34</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>-0.1245</v>
+        <v>-0.3375</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>-0.122</v>
+        <v>-0.335</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>-0.1195</v>
+        <v>-0.3325</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>-0.117</v>
+        <v>-0.33</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>-0.1145</v>
+        <v>-0.3275</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -554,15 +554,15 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>-0.112</v>
+        <v>-0.325</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>-0.1095</v>
+        <v>-0.3225</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>-0.107</v>
+        <v>-0.32</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -578,7 +578,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>-0.1045</v>
+        <v>-0.3175</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>-0.102</v>
+        <v>-0.315</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>-0.09950000000000001</v>
+        <v>-0.3125</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>-0.097</v>
+        <v>-0.31</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>-0.0945</v>
+        <v>-0.3075</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>-0.092</v>
+        <v>-0.305</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>-0.0895</v>
+        <v>-0.3025</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>-0.08699999999999999</v>
+        <v>-0.3</v>
       </c>
       <c r="B26" t="n">
         <v>0</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>-0.08450000000000001</v>
+        <v>-0.2975</v>
       </c>
       <c r="B27" t="n">
         <v>0</v>
@@ -650,7 +650,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>-0.082</v>
+        <v>-0.295</v>
       </c>
       <c r="B28" t="n">
         <v>0</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>-0.0795</v>
+        <v>-0.2925</v>
       </c>
       <c r="B29" t="n">
         <v>0</v>
@@ -666,15 +666,15 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>-0.077</v>
+        <v>-0.29</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>-0.0745</v>
+        <v>-0.2875</v>
       </c>
       <c r="B31" t="n">
         <v>0</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>-0.07199999999999999</v>
+        <v>-0.285</v>
       </c>
       <c r="B32" t="n">
         <v>0</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>-0.06950000000000001</v>
+        <v>-0.2825</v>
       </c>
       <c r="B33" t="n">
         <v>0</v>
@@ -698,7 +698,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>-0.067</v>
+        <v>-0.28</v>
       </c>
       <c r="B34" t="n">
         <v>0</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>-0.0645</v>
+        <v>-0.2775</v>
       </c>
       <c r="B35" t="n">
         <v>0</v>
@@ -714,7 +714,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>-0.062</v>
+        <v>-0.275</v>
       </c>
       <c r="B36" t="n">
         <v>0</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>-0.0595</v>
+        <v>-0.2725</v>
       </c>
       <c r="B37" t="n">
         <v>0</v>
@@ -730,7 +730,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>-0.057</v>
+        <v>-0.27</v>
       </c>
       <c r="B38" t="n">
         <v>0</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>-0.0545</v>
+        <v>-0.2675</v>
       </c>
       <c r="B39" t="n">
         <v>0</v>
@@ -746,15 +746,15 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>-0.052</v>
+        <v>-0.265</v>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>-0.0495</v>
+        <v>-0.2625</v>
       </c>
       <c r="B41" t="n">
         <v>0</v>
@@ -762,7 +762,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>-0.047</v>
+        <v>-0.26</v>
       </c>
       <c r="B42" t="n">
         <v>0</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>-0.0445</v>
+        <v>-0.2575</v>
       </c>
       <c r="B43" t="n">
         <v>0</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>-0.042</v>
+        <v>-0.255</v>
       </c>
       <c r="B44" t="n">
         <v>0</v>
@@ -786,7 +786,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>-0.0395</v>
+        <v>-0.2525</v>
       </c>
       <c r="B45" t="n">
         <v>0</v>
@@ -794,15 +794,15 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>-0.037</v>
+        <v>-0.25</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>-0.0345</v>
+        <v>-0.2475</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>-0.032</v>
+        <v>-0.245</v>
       </c>
       <c r="B48" t="n">
         <v>0</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>-0.0295</v>
+        <v>-0.2425</v>
       </c>
       <c r="B49" t="n">
         <v>0</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>-0.027</v>
+        <v>-0.24</v>
       </c>
       <c r="B50" t="n">
         <v>0</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>-0.0245</v>
+        <v>-0.2375</v>
       </c>
       <c r="B51" t="n">
         <v>0</v>
@@ -842,15 +842,15 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>-0.022</v>
+        <v>-0.235</v>
       </c>
       <c r="B52" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>-0.0195</v>
+        <v>-0.2325</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>-0.017</v>
+        <v>-0.23</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>-0.0145</v>
+        <v>-0.2275</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>-0.012</v>
+        <v>-0.225</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
@@ -882,7 +882,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>-0.0095</v>
+        <v>-0.2225</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
@@ -890,15 +890,15 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>-0.007</v>
+        <v>-0.22</v>
       </c>
       <c r="B58" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>-0.0045</v>
+        <v>-0.2175</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>-0.002</v>
+        <v>-0.215</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>0.0005</v>
+        <v>-0.2125</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
@@ -922,15 +922,15 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>0.003</v>
+        <v>-0.21</v>
       </c>
       <c r="B62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>0.0055</v>
+        <v>-0.2075</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>0.008</v>
+        <v>-0.205</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>0.0105</v>
+        <v>-0.2025</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
@@ -954,15 +954,15 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>0.013</v>
+        <v>-0.2</v>
       </c>
       <c r="B66" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>0.0155</v>
+        <v>-0.1975</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
@@ -970,15 +970,15 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>0.018</v>
+        <v>-0.195</v>
       </c>
       <c r="B68" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>0.0205</v>
+        <v>-0.1925</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>0.023</v>
+        <v>-0.19</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>0.0255</v>
+        <v>-0.1875</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
@@ -1002,7 +1002,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>0.028</v>
+        <v>-0.185</v>
       </c>
       <c r="B72" t="n">
         <v>1</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>0.0305</v>
+        <v>-0.1825</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
@@ -1018,15 +1018,15 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>0.033</v>
+        <v>-0.18</v>
       </c>
       <c r="B74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>0.0355</v>
+        <v>-0.1775</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>0.038</v>
+        <v>-0.175</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>0.0405</v>
+        <v>-0.1725</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
@@ -1050,9 +1050,1449 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>0.043</v>
+        <v>-0.17</v>
       </c>
       <c r="B78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>-0.1675</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>-0.165</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>-0.1625</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>-0.16</v>
+      </c>
+      <c r="B82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>-0.1575</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>-0.155</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>-0.1525</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>-0.15</v>
+      </c>
+      <c r="B86" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>-0.1475</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>-0.145</v>
+      </c>
+      <c r="B88" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>-0.1425</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>-0.1375</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>-0.135</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>-0.1325</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>-0.13</v>
+      </c>
+      <c r="B94" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>-0.1275</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>-0.125</v>
+      </c>
+      <c r="B96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>-0.1225</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="B98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>-0.1175</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>-0.115</v>
+      </c>
+      <c r="B100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>-0.1125</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="B102" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>-0.1075</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>-0.105</v>
+      </c>
+      <c r="B104" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>-0.1025</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="B106" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>-0.0975</v>
+      </c>
+      <c r="B107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>-0.095</v>
+      </c>
+      <c r="B108" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>-0.0925</v>
+      </c>
+      <c r="B109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="B110" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>-0.08749999999999999</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>-0.08500000000000001</v>
+      </c>
+      <c r="B112" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>-0.0825</v>
+      </c>
+      <c r="B113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="B114" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>-0.0775</v>
+      </c>
+      <c r="B115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>-0.075</v>
+      </c>
+      <c r="B116" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>-0.0725</v>
+      </c>
+      <c r="B117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="B118" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>-0.0675</v>
+      </c>
+      <c r="B119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>-0.065</v>
+      </c>
+      <c r="B120" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>-0.0625</v>
+      </c>
+      <c r="B121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="B122" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>-0.0575</v>
+      </c>
+      <c r="B123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>-0.055</v>
+      </c>
+      <c r="B124" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>-0.0525</v>
+      </c>
+      <c r="B125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="B126" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>-0.0475</v>
+      </c>
+      <c r="B127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>-0.045</v>
+      </c>
+      <c r="B128" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>-0.0425</v>
+      </c>
+      <c r="B129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="B130" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>-0.0375</v>
+      </c>
+      <c r="B131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>-0.035</v>
+      </c>
+      <c r="B132" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>-0.0325</v>
+      </c>
+      <c r="B133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="B134" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>-0.0275</v>
+      </c>
+      <c r="B135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>-0.025</v>
+      </c>
+      <c r="B136" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>-0.0225</v>
+      </c>
+      <c r="B137" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="B138" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>-0.0175</v>
+      </c>
+      <c r="B139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>-0.015</v>
+      </c>
+      <c r="B140" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>-0.0125</v>
+      </c>
+      <c r="B141" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="B142" t="n">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>-0.0075</v>
+      </c>
+      <c r="B143" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="B144" t="n">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>-0.0025</v>
+      </c>
+      <c r="B145" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B146" t="n">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>0.0025</v>
+      </c>
+      <c r="B147" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="B148" t="n">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>0.0075</v>
+      </c>
+      <c r="B149" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="B150" t="n">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>0.0125</v>
+      </c>
+      <c r="B151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="B152" t="n">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>0.0175</v>
+      </c>
+      <c r="B153" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="B154" t="n">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>0.0225</v>
+      </c>
+      <c r="B155" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="B156" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>0.0275</v>
+      </c>
+      <c r="B157" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="B158" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>0.0325</v>
+      </c>
+      <c r="B159" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="B160" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>0.0375</v>
+      </c>
+      <c r="B161" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="B162" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>0.0425</v>
+      </c>
+      <c r="B163" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="B164" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>0.0475</v>
+      </c>
+      <c r="B165" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="B166" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>0.0525</v>
+      </c>
+      <c r="B167" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="B168" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>0.0575</v>
+      </c>
+      <c r="B169" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="B170" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="B171" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="B172" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>0.0675</v>
+      </c>
+      <c r="B173" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="B174" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>0.0725</v>
+      </c>
+      <c r="B175" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="B176" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>0.0775</v>
+      </c>
+      <c r="B177" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="B178" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>0.0825</v>
+      </c>
+      <c r="B179" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="B180" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>0.08749999999999999</v>
+      </c>
+      <c r="B181" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="B182" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>0.0925</v>
+      </c>
+      <c r="B183" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="B184" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>0.0975</v>
+      </c>
+      <c r="B185" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B186" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>0.1025</v>
+      </c>
+      <c r="B187" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="B188" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>0.1075</v>
+      </c>
+      <c r="B189" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="B190" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>0.1125</v>
+      </c>
+      <c r="B191" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>0.115</v>
+      </c>
+      <c r="B192" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>0.1175</v>
+      </c>
+      <c r="B193" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="B194" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>0.1225</v>
+      </c>
+      <c r="B195" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="B196" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>0.1275</v>
+      </c>
+      <c r="B197" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="B198" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>0.1325</v>
+      </c>
+      <c r="B199" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="B200" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>0.1375</v>
+      </c>
+      <c r="B201" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="B202" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>0.1425</v>
+      </c>
+      <c r="B203" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="B204" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>0.1475</v>
+      </c>
+      <c r="B205" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="B206" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>0.1525</v>
+      </c>
+      <c r="B207" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="B208" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>0.1575</v>
+      </c>
+      <c r="B209" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="B210" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>0.1625</v>
+      </c>
+      <c r="B211" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="B212" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>0.1675</v>
+      </c>
+      <c r="B213" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="B214" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>0.1725</v>
+      </c>
+      <c r="B215" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="B216" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>0.1775</v>
+      </c>
+      <c r="B217" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="B218" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>0.1825</v>
+      </c>
+      <c r="B219" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>0.185</v>
+      </c>
+      <c r="B220" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>0.1875</v>
+      </c>
+      <c r="B221" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="B222" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>0.1925</v>
+      </c>
+      <c r="B223" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>0.195</v>
+      </c>
+      <c r="B224" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>0.1975</v>
+      </c>
+      <c r="B225" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B226" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>0.2025</v>
+      </c>
+      <c r="B227" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="B228" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>0.2075</v>
+      </c>
+      <c r="B229" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="B230" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>0.2125</v>
+      </c>
+      <c r="B231" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>0.215</v>
+      </c>
+      <c r="B232" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>0.2175</v>
+      </c>
+      <c r="B233" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="B234" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>0.2225</v>
+      </c>
+      <c r="B235" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="B236" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>0.2275</v>
+      </c>
+      <c r="B237" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="B238" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>0.2325</v>
+      </c>
+      <c r="B239" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>0.235</v>
+      </c>
+      <c r="B240" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="n">
+        <v>0.2375</v>
+      </c>
+      <c r="B241" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="B242" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>0.2425</v>
+      </c>
+      <c r="B243" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>0.245</v>
+      </c>
+      <c r="B244" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>0.2475</v>
+      </c>
+      <c r="B245" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B246" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="n">
+        <v>0.2525</v>
+      </c>
+      <c r="B247" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="n">
+        <v>0.255</v>
+      </c>
+      <c r="B248" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="n">
+        <v>0.2575</v>
+      </c>
+      <c r="B249" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="B250" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n">
+        <v>0.2625</v>
+      </c>
+      <c r="B251" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>0.265</v>
+      </c>
+      <c r="B252" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n">
+        <v>0.2675</v>
+      </c>
+      <c r="B253" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="B254" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n">
+        <v>0.2725</v>
+      </c>
+      <c r="B255" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="B256" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="n">
+        <v>0.2775</v>
+      </c>
+      <c r="B257" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="B258" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>